<commit_message>
Update the metadata template for transcriptomics.
</commit_message>
<xml_diff>
--- a/docs/assets/templates/2022051201_transcriptomics-metadata-template_chinese.xlsx
+++ b/docs/assets/templates/2022051201_transcriptomics-metadata-template_chinese.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codespace/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845A422B-1AD7-ED46-AB20-05A97DDEEF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C46765B-69B2-684E-A95A-98A858ABA96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1500" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{A58EA485-3F1D-4B3F-B94B-7C41644033AE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{A58EA485-3F1D-4B3F-B94B-7C41644033AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Please Read First!" sheetId="5" r:id="rId1"/>
-    <sheet name="metadata" sheetId="4" r:id="rId2"/>
-    <sheet name="quality_control" sheetId="6" r:id="rId3"/>
+    <sheet name="analysis_pipeline" sheetId="7" r:id="rId2"/>
+    <sheet name="metadata" sheetId="4" r:id="rId3"/>
+    <sheet name="quality_control" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="321">
   <si>
     <t>sample_id</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -960,12 +961,304 @@
   <si>
     <t>测序总读段数，单位是M</t>
   </si>
+  <si>
+    <t>Sheet - Analysis Pipeline</t>
+  </si>
+  <si>
+    <t>reference_genome</t>
+  </si>
+  <si>
+    <t>参考基因组</t>
+  </si>
+  <si>
+    <t>Reference genome</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>GRCh38 (hg38)</t>
+  </si>
+  <si>
+    <t>只有一种选项:GRCh38 (hg38)</t>
+  </si>
+  <si>
+    <t>source_gene_annotation</t>
+  </si>
+  <si>
+    <t>基因注释来源</t>
+  </si>
+  <si>
+    <t>Source of gene annotation</t>
+  </si>
+  <si>
+    <t>基因模型来源，例如Ensembl, UCSC, RefSeq等，基因模型文件通常是gtf/gff格式</t>
+  </si>
+  <si>
+    <t>Ensembl</t>
+  </si>
+  <si>
+    <r>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个选项：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ensembl, UCSC, RefSeq, GENCODE, other</t>
+    </r>
+  </si>
+  <si>
+    <t>gene_annotation_version</t>
+  </si>
+  <si>
+    <t>基因注释版本</t>
+  </si>
+  <si>
+    <t>Version of gene anntation</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>gene_naming_category</t>
+  </si>
+  <si>
+    <t>基因命名种类</t>
+  </si>
+  <si>
+    <t>Category of gene naming</t>
+  </si>
+  <si>
+    <t>Ensembl ID</t>
+  </si>
+  <si>
+    <r>
+      <t>4个选项：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ensembl ID, HGNC symbol, Entrez ID, other</t>
+    </r>
+  </si>
+  <si>
+    <t>alignment_software</t>
+  </si>
+  <si>
+    <t>比对软件</t>
+  </si>
+  <si>
+    <t>Software(s) that is (are) used for aligning reads to reference genome, using semicolons (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>用于将序列比对至参考基因组软件，如果使用多个比对软件，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t>Alignment</t>
+  </si>
+  <si>
+    <t>HISAT2</t>
+  </si>
+  <si>
+    <t>alignment_software_version</t>
+  </si>
+  <si>
+    <t>比对软件版本号</t>
+  </si>
+  <si>
+    <t>Alignment software version(s), using semicolons (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>比对软件版本号，如果使用多个比对软件，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> v0.11.5</t>
+  </si>
+  <si>
+    <t>alignment_command</t>
+  </si>
+  <si>
+    <t>比对软件命令行</t>
+  </si>
+  <si>
+    <t>Command(s) of alignment, using semicolons (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>比对运行命令行，如果使用多行命令，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hisat2 -p 8 -x reference/References_GRCh38/GRCh38/ -1 sample_R1.fastq.gz -2 sample_R2.fastq.gz -S sample.sam </t>
+  </si>
+  <si>
+    <t>quantification_software</t>
+  </si>
+  <si>
+    <t>定量软件</t>
+  </si>
+  <si>
+    <t>Software(s) that is (are) used for quantification to gene models, using semicolons (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>定量软件，如果使用多个软件，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t>Quantification</t>
+  </si>
+  <si>
+    <t>StringTie</t>
+  </si>
+  <si>
+    <t>quantification_software_version</t>
+  </si>
+  <si>
+    <t>定量软件版本号</t>
+  </si>
+  <si>
+    <t>Quantification software version(s), using semicolons (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>定量软件版本号，如果使用多个软件，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t>v1.3.4</t>
+  </si>
+  <si>
+    <t>quantification_command</t>
+  </si>
+  <si>
+    <t>定量软件命令行</t>
+  </si>
+  <si>
+    <t>Command(s) of quantification, using semicolons (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>定量软件命令行，如果使用多个软件，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t>stringtie -e -B -p 8 -G Homo_sapiens.GRCh38.93.gtf  -g sample_genecount.csv -o sample.gtf -C sample.cov.ref.gtf -A sample.gene.abundance.txt sample.sorted.bam</t>
+  </si>
+  <si>
+    <t>quality_control_software</t>
+  </si>
+  <si>
+    <t>质控软件</t>
+  </si>
+  <si>
+    <t>Software(s) that is (are) used for quality control (QC), using semicolons (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>质控软件，如果使用多个软件，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>FastQC</t>
+  </si>
+  <si>
+    <t>quality_control_software_version</t>
+  </si>
+  <si>
+    <t>质控软件版本号</t>
+  </si>
+  <si>
+    <t>QC software version(s), using semicolons (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>质控软件版本号，如果使用多个软件，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t>quality_control_command</t>
+  </si>
+  <si>
+    <t>质控软件命令行</t>
+  </si>
+  <si>
+    <t>Command(s) of QC, using semicolons (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>质控软件命令行，如果使用多个软件，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t>fastqc –o outdir sample.fastq.gz</t>
+  </si>
+  <si>
+    <t>other_software</t>
+  </si>
+  <si>
+    <t>其它软件</t>
+  </si>
+  <si>
+    <t>Other software(s), using (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>其它软件，如果使用多个软件，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>other_software_purpose</t>
+  </si>
+  <si>
+    <t>其它软件用途</t>
+  </si>
+  <si>
+    <t>The purpose of software(s), using (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>其它软件用途，如果使用多个软件，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t>other_software_version</t>
+  </si>
+  <si>
+    <t>其它软件版本号</t>
+  </si>
+  <si>
+    <t>Software version(s), using semicolons (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>其它软件版本号，如果使用多个软件，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t>other_command</t>
+  </si>
+  <si>
+    <t>其它软件命令行</t>
+  </si>
+  <si>
+    <t>Command(s) of software, using semicolons (;) to separate if contains multiple softwares</t>
+  </si>
+  <si>
+    <t>其它软件命令行，如果使用多个软件，则用分号分隔 (;)</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31">
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1162,8 +1455,39 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1206,8 +1530,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDEDED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1245,6 +1599,93 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1253,7 +1694,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1443,6 +1884,45 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1452,47 +1932,98 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1810,99 +2341,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F19F2F-4205-8046-8351-0FE58B3231A2}">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J3"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.6640625" defaultRowHeight="24" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="30" style="15" customWidth="1"/>
+    <col min="1" max="1" width="30" style="15" customWidth="1"/>
+    <col min="2" max="2" width="30" style="58" customWidth="1"/>
     <col min="3" max="3" width="41.6640625" style="17" customWidth="1"/>
     <col min="4" max="4" width="34.83203125" style="57" customWidth="1"/>
     <col min="5" max="5" width="32.33203125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" style="57" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" style="57" customWidth="1"/>
     <col min="7" max="7" width="23.6640625" style="17" customWidth="1"/>
-    <col min="8" max="8" width="38.83203125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" style="17" customWidth="1"/>
     <col min="9" max="9" width="21.83203125" style="17" customWidth="1"/>
     <col min="10" max="10" width="23" style="17" customWidth="1"/>
     <col min="11" max="16384" width="34.6640625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" ht="33" customHeight="1">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="71" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
     </row>
     <row r="2" spans="1:10" s="8" customFormat="1" ht="47" customHeight="1">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="72" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
     </row>
     <row r="3" spans="1:10" s="8" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10" s="8" customFormat="1" ht="24" customHeight="1">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
     </row>
     <row r="5" spans="1:10" s="8" customFormat="1" ht="24" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="59" t="s">
         <v>210</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="59" t="s">
         <v>209</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="63" t="s">
+      <c r="F5" s="59" t="s">
         <v>213</v>
       </c>
       <c r="G5" s="10" t="s">
@@ -1922,19 +2454,19 @@
       <c r="A6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="60" t="s">
         <v>158</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="69" t="s">
+      <c r="D6" s="65" t="s">
         <v>158</v>
       </c>
       <c r="E6" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="70" t="s">
+      <c r="F6" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -1948,19 +2480,19 @@
       <c r="A7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="60" t="s">
         <v>159</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="65" t="s">
         <v>159</v>
       </c>
       <c r="E7" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="70" t="s">
+      <c r="F7" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G7" s="8" t="s">
@@ -1977,19 +2509,19 @@
       <c r="A8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="60" t="s">
         <v>160</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="69" t="s">
+      <c r="D8" s="65" t="s">
         <v>204</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="70" t="s">
+      <c r="F8" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G8" s="8" t="s">
@@ -2003,19 +2535,19 @@
       <c r="A9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="60" t="s">
         <v>161</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="69" t="s">
+      <c r="D9" s="65" t="s">
         <v>161</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F9" s="70" t="s">
+      <c r="F9" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G9" s="8" t="s">
@@ -2029,19 +2561,19 @@
       <c r="A10" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="61" t="s">
         <v>162</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="65" t="s">
         <v>162</v>
       </c>
       <c r="E10" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="70" t="s">
+      <c r="F10" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G10" s="8" t="s">
@@ -2055,19 +2587,19 @@
       <c r="A11" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="61" t="s">
         <v>163</v>
       </c>
       <c r="C11" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="65" t="s">
+      <c r="D11" s="61" t="s">
         <v>163</v>
       </c>
       <c r="E11" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F11" s="70" t="s">
+      <c r="F11" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G11" s="8" t="s">
@@ -2081,19 +2613,19 @@
       <c r="A12" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="62" t="s">
         <v>164</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D12" s="62" t="s">
         <v>164</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="70" t="s">
+      <c r="F12" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G12" s="8" t="s">
@@ -2107,19 +2639,19 @@
       <c r="A13" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="62" t="s">
         <v>165</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="66" t="s">
+      <c r="D13" s="62" t="s">
         <v>165</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="70" t="s">
+      <c r="F13" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G13" s="8" t="s">
@@ -2136,19 +2668,19 @@
       <c r="A14" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="62" t="s">
         <v>166</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D14" s="66" t="s">
+      <c r="D14" s="62" t="s">
         <v>166</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="70" t="s">
+      <c r="F14" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G14" s="8" t="s">
@@ -2162,19 +2694,19 @@
       <c r="A15" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="62" t="s">
         <v>167</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="66" t="s">
+      <c r="D15" s="62" t="s">
         <v>167</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="70" t="s">
+      <c r="F15" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G15" s="8" t="s">
@@ -2188,19 +2720,19 @@
       <c r="A16" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="62" t="s">
         <v>168</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="66" t="s">
+      <c r="D16" s="62" t="s">
         <v>168</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="70" t="s">
+      <c r="F16" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G16" s="8" t="s">
@@ -2214,19 +2746,19 @@
       <c r="A17" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="62" t="s">
         <v>169</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="66" t="s">
+      <c r="D17" s="62" t="s">
         <v>205</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="71" t="s">
+      <c r="F17" s="67" t="s">
         <v>212</v>
       </c>
       <c r="G17" s="17" t="s">
@@ -2237,19 +2769,19 @@
       <c r="A18" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="63" t="s">
         <v>170</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="66" t="s">
+      <c r="D18" s="62" t="s">
         <v>170</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="70" t="s">
+      <c r="F18" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G18" s="17" t="s">
@@ -2263,19 +2795,19 @@
       <c r="A19" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="67" t="s">
+      <c r="B19" s="63" t="s">
         <v>171</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="66" t="s">
+      <c r="D19" s="62" t="s">
         <v>171</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="71" t="s">
+      <c r="F19" s="67" t="s">
         <v>212</v>
       </c>
       <c r="G19" s="17" t="s">
@@ -2289,19 +2821,19 @@
       <c r="A20" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="62" t="s">
         <v>172</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="66" t="s">
+      <c r="D20" s="62" t="s">
         <v>206</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="70" t="s">
+      <c r="F20" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G20" s="17" t="s">
@@ -2315,19 +2847,19 @@
       <c r="A21" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="62" t="s">
         <v>173</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="66" t="s">
+      <c r="D21" s="62" t="s">
         <v>207</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="70" t="s">
+      <c r="F21" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G21" s="17" t="s">
@@ -2341,19 +2873,19 @@
       <c r="A22" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="62" t="s">
         <v>174</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="66" t="s">
+      <c r="D22" s="62" t="s">
         <v>208</v>
       </c>
       <c r="E22" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="70" t="s">
+      <c r="F22" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G22" s="17" t="s">
@@ -2367,19 +2899,19 @@
       <c r="A23" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="62" t="s">
         <v>175</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="D23" s="66" t="s">
+      <c r="D23" s="62" t="s">
         <v>175</v>
       </c>
       <c r="E23" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F23" s="70" t="s">
+      <c r="F23" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G23" s="17" t="s">
@@ -2393,19 +2925,19 @@
       <c r="A24" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="62" t="s">
         <v>176</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="66" t="s">
+      <c r="D24" s="62" t="s">
         <v>176</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="70" t="s">
+      <c r="F24" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G24" s="17" t="s">
@@ -2419,19 +2951,19 @@
       <c r="A25" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="62" t="s">
         <v>177</v>
       </c>
       <c r="C25" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D25" s="66" t="s">
+      <c r="D25" s="62" t="s">
         <v>177</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F25" s="70" t="s">
+      <c r="F25" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G25" s="40" t="s">
@@ -2445,19 +2977,19 @@
       <c r="A26" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="62" t="s">
         <v>178</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="66" t="s">
+      <c r="D26" s="62" t="s">
         <v>178</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F26" s="70" t="s">
+      <c r="F26" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G26" s="17" t="s">
@@ -2471,19 +3003,19 @@
       <c r="A27" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="62" t="s">
         <v>179</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="66" t="s">
+      <c r="D27" s="62" t="s">
         <v>179</v>
       </c>
       <c r="E27" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F27" s="70" t="s">
+      <c r="F27" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G27" s="17" t="s">
@@ -2497,19 +3029,19 @@
       <c r="A28" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="66" t="s">
+      <c r="B28" s="62" t="s">
         <v>180</v>
       </c>
       <c r="C28" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="66" t="s">
+      <c r="D28" s="62" t="s">
         <v>180</v>
       </c>
       <c r="E28" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="71" t="s">
+      <c r="F28" s="67" t="s">
         <v>212</v>
       </c>
       <c r="G28" s="17" t="s">
@@ -2520,19 +3052,19 @@
       <c r="A29" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="62" t="s">
         <v>181</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="66" t="s">
+      <c r="D29" s="62" t="s">
         <v>181</v>
       </c>
       <c r="E29" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="70" t="s">
+      <c r="F29" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G29" s="17" t="s">
@@ -2546,19 +3078,19 @@
       <c r="A30" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="62" t="s">
         <v>182</v>
       </c>
       <c r="C30" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D30" s="66" t="s">
+      <c r="D30" s="62" t="s">
         <v>182</v>
       </c>
       <c r="E30" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F30" s="70" t="s">
+      <c r="F30" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G30" s="17" t="s">
@@ -2572,19 +3104,19 @@
       <c r="A31" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="66" t="s">
+      <c r="B31" s="62" t="s">
         <v>183</v>
       </c>
       <c r="C31" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="66" t="s">
+      <c r="D31" s="62" t="s">
         <v>183</v>
       </c>
       <c r="E31" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="70" t="s">
+      <c r="F31" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G31" s="17" t="s">
@@ -2598,19 +3130,19 @@
       <c r="A32" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="66" t="s">
+      <c r="B32" s="62" t="s">
         <v>184</v>
       </c>
       <c r="C32" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="D32" s="66" t="s">
+      <c r="D32" s="62" t="s">
         <v>184</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F32" s="70" t="s">
+      <c r="F32" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G32" s="17" t="s">
@@ -2624,19 +3156,19 @@
       <c r="A33" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="66" t="s">
+      <c r="B33" s="62" t="s">
         <v>185</v>
       </c>
       <c r="C33" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D33" s="66" t="s">
+      <c r="D33" s="62" t="s">
         <v>185</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F33" s="70" t="s">
+      <c r="F33" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G33" s="17" t="s">
@@ -2650,19 +3182,19 @@
       <c r="A34" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="66" t="s">
+      <c r="B34" s="62" t="s">
         <v>186</v>
       </c>
       <c r="C34" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="66" t="s">
+      <c r="D34" s="62" t="s">
         <v>186</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F34" s="70" t="s">
+      <c r="F34" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G34" s="17" t="s">
@@ -2676,19 +3208,19 @@
       <c r="A35" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="66" t="s">
+      <c r="B35" s="62" t="s">
         <v>187</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="66" t="s">
+      <c r="D35" s="62" t="s">
         <v>187</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F35" s="70" t="s">
+      <c r="F35" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G35" s="17" t="s">
@@ -2702,19 +3234,19 @@
       <c r="A36" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="66" t="s">
+      <c r="B36" s="62" t="s">
         <v>188</v>
       </c>
       <c r="C36" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="66" t="s">
+      <c r="D36" s="62" t="s">
         <v>188</v>
       </c>
       <c r="E36" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F36" s="70" t="s">
+      <c r="F36" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G36" s="17" t="s">
@@ -2728,19 +3260,19 @@
       <c r="A37" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="66" t="s">
+      <c r="B37" s="62" t="s">
         <v>170</v>
       </c>
       <c r="C37" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D37" s="66" t="s">
+      <c r="D37" s="62" t="s">
         <v>170</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F37" s="70" t="s">
+      <c r="F37" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G37" s="40" t="s">
@@ -2754,19 +3286,19 @@
       <c r="A38" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="66" t="s">
+      <c r="B38" s="62" t="s">
         <v>171</v>
       </c>
       <c r="C38" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D38" s="66" t="s">
+      <c r="D38" s="62" t="s">
         <v>171</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F38" s="71" t="s">
+      <c r="F38" s="67" t="s">
         <v>212</v>
       </c>
       <c r="G38" s="17" t="s">
@@ -2780,19 +3312,19 @@
       <c r="A39" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="B39" s="66" t="s">
+      <c r="B39" s="62" t="s">
         <v>189</v>
       </c>
       <c r="C39" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D39" s="66" t="s">
+      <c r="D39" s="62" t="s">
         <v>189</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F39" s="71" t="s">
+      <c r="F39" s="67" t="s">
         <v>212</v>
       </c>
       <c r="G39" s="17" t="s">
@@ -2806,19 +3338,19 @@
       <c r="A40" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="66" t="s">
+      <c r="B40" s="62" t="s">
         <v>190</v>
       </c>
       <c r="C40" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="66" t="s">
+      <c r="D40" s="62" t="s">
         <v>190</v>
       </c>
       <c r="E40" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F40" s="71" t="s">
+      <c r="F40" s="67" t="s">
         <v>212</v>
       </c>
       <c r="G40" s="17" t="s">
@@ -2832,19 +3364,19 @@
       <c r="A41" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="66" t="s">
+      <c r="B41" s="62" t="s">
         <v>191</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="66" t="s">
+      <c r="D41" s="62" t="s">
         <v>191</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F41" s="70" t="s">
+      <c r="F41" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G41" s="17" t="s">
@@ -2858,19 +3390,19 @@
       <c r="A42" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="66" t="s">
+      <c r="B42" s="62" t="s">
         <v>192</v>
       </c>
       <c r="C42" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D42" s="66" t="s">
+      <c r="D42" s="62" t="s">
         <v>192</v>
       </c>
       <c r="E42" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F42" s="70" t="s">
+      <c r="F42" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G42" s="17" t="s">
@@ -2884,19 +3416,19 @@
       <c r="A43" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="B43" s="66" t="s">
+      <c r="B43" s="62" t="s">
         <v>175</v>
       </c>
       <c r="C43" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="D43" s="66" t="s">
+      <c r="D43" s="62" t="s">
         <v>175</v>
       </c>
       <c r="E43" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F43" s="70" t="s">
+      <c r="F43" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G43" s="17" t="s">
@@ -2910,19 +3442,19 @@
       <c r="A44" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="68" t="s">
+      <c r="B44" s="64" t="s">
         <v>193</v>
       </c>
       <c r="C44" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="D44" s="68" t="s">
+      <c r="D44" s="64" t="s">
         <v>193</v>
       </c>
       <c r="E44" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F44" s="70" t="s">
+      <c r="F44" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G44" s="17" t="s">
@@ -2939,19 +3471,19 @@
       <c r="A45" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="66" t="s">
+      <c r="B45" s="62" t="s">
         <v>194</v>
       </c>
       <c r="C45" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="D45" s="66" t="s">
+      <c r="D45" s="62" t="s">
         <v>194</v>
       </c>
       <c r="E45" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F45" s="70" t="s">
+      <c r="F45" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G45" s="17" t="s">
@@ -2965,19 +3497,19 @@
       <c r="A46" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="68" t="s">
+      <c r="B46" s="64" t="s">
         <v>195</v>
       </c>
       <c r="C46" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="D46" s="68" t="s">
+      <c r="D46" s="64" t="s">
         <v>195</v>
       </c>
       <c r="E46" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F46" s="70" t="s">
+      <c r="F46" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G46" s="17" t="s">
@@ -2991,19 +3523,19 @@
       <c r="A47" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="66" t="s">
+      <c r="B47" s="62" t="s">
         <v>196</v>
       </c>
       <c r="C47" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="D47" s="66" t="s">
+      <c r="D47" s="62" t="s">
         <v>196</v>
       </c>
       <c r="E47" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F47" s="70" t="s">
+      <c r="F47" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G47" s="17" t="s">
@@ -3017,19 +3549,19 @@
       <c r="A48" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B48" s="66" t="s">
+      <c r="B48" s="62" t="s">
         <v>197</v>
       </c>
       <c r="C48" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="D48" s="66" t="s">
+      <c r="D48" s="62" t="s">
         <v>197</v>
       </c>
       <c r="E48" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F48" s="70" t="s">
+      <c r="F48" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G48" s="17" t="s">
@@ -3039,43 +3571,43 @@
         <v>20028312</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="24" customHeight="1">
+    <row r="49" spans="1:10" ht="24" customHeight="1">
       <c r="A49" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="66" t="s">
+      <c r="B49" s="62" t="s">
         <v>198</v>
       </c>
       <c r="C49" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="D49" s="66" t="s">
+      <c r="D49" s="62" t="s">
         <v>198</v>
       </c>
       <c r="E49" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F49" s="71" t="s">
+      <c r="F49" s="67" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="24" customHeight="1">
+    <row r="50" spans="1:10" ht="24" customHeight="1">
       <c r="A50" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="66" t="s">
+      <c r="B50" s="62" t="s">
         <v>199</v>
       </c>
       <c r="C50" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="D50" s="66" t="s">
+      <c r="D50" s="62" t="s">
         <v>199</v>
       </c>
       <c r="E50" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F50" s="70" t="s">
+      <c r="F50" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G50" s="17" t="s">
@@ -3085,23 +3617,23 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="24" customHeight="1">
+    <row r="51" spans="1:10" ht="24" customHeight="1">
       <c r="A51" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="66" t="s">
+      <c r="B51" s="62" t="s">
         <v>200</v>
       </c>
       <c r="C51" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="D51" s="66" t="s">
+      <c r="D51" s="62" t="s">
         <v>200</v>
       </c>
       <c r="E51" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F51" s="70" t="s">
+      <c r="F51" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G51" s="17" t="s">
@@ -3111,69 +3643,69 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="24" customHeight="1">
+    <row r="52" spans="1:10" ht="24" customHeight="1">
       <c r="A52" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="66" t="s">
+      <c r="B52" s="62" t="s">
         <v>201</v>
       </c>
       <c r="C52" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="D52" s="66" t="s">
+      <c r="D52" s="62" t="s">
         <v>201</v>
       </c>
       <c r="E52" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F52" s="70" t="s">
+      <c r="F52" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G52" s="17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="24" customHeight="1">
+    <row r="53" spans="1:10" ht="24" customHeight="1">
       <c r="A53" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="66" t="s">
+      <c r="B53" s="62" t="s">
         <v>202</v>
       </c>
       <c r="C53" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="D53" s="66" t="s">
+      <c r="D53" s="62" t="s">
         <v>202</v>
       </c>
       <c r="E53" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F53" s="70" t="s">
+      <c r="F53" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G53" s="17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="24" customHeight="1">
+    <row r="54" spans="1:10" ht="24" customHeight="1">
       <c r="A54" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="66" t="s">
+      <c r="B54" s="62" t="s">
         <v>203</v>
       </c>
       <c r="C54" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="D54" s="66" t="s">
+      <c r="D54" s="62" t="s">
         <v>203</v>
       </c>
       <c r="E54" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F54" s="70" t="s">
+      <c r="F54" s="66" t="s">
         <v>211</v>
       </c>
       <c r="G54" s="22" t="s">
@@ -3183,32 +3715,35 @@
         <v>20200808</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="24" customHeight="1">
+    <row r="55" spans="1:10" ht="24" customHeight="1">
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
       <c r="E55" s="22"/>
       <c r="F55" s="22"/>
     </row>
-    <row r="56" spans="1:9" ht="24" customHeight="1">
+    <row r="56" spans="1:10" ht="24" customHeight="1">
       <c r="C56" s="22"/>
       <c r="D56" s="22"/>
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
-    </row>
-    <row r="57" spans="1:9" ht="24" customHeight="1">
-      <c r="A57" s="61" t="s">
+      <c r="G56" s="58"/>
+      <c r="H56" s="58"/>
+      <c r="I56" s="58"/>
+    </row>
+    <row r="57" spans="1:10" ht="24" customHeight="1">
+      <c r="A57" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="61"/>
-      <c r="C57" s="61"/>
-      <c r="D57" s="61"/>
-      <c r="E57" s="61"/>
-      <c r="F57" s="61"/>
-      <c r="G57" s="61"/>
-      <c r="H57" s="61"/>
-      <c r="I57" s="61"/>
-    </row>
-    <row r="58" spans="1:9" ht="24" customHeight="1">
+      <c r="B57" s="90"/>
+      <c r="C57" s="90"/>
+      <c r="D57" s="90"/>
+      <c r="E57" s="90"/>
+      <c r="F57" s="90"/>
+      <c r="G57" s="90"/>
+      <c r="H57" s="90"/>
+      <c r="I57" s="91"/>
+    </row>
+    <row r="58" spans="1:10" ht="24" customHeight="1">
       <c r="A58" s="9" t="s">
         <v>5</v>
       </c>
@@ -3236,207 +3771,216 @@
       <c r="I58" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="24" customHeight="1">
+      <c r="J58" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="24" customHeight="1">
       <c r="A59" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="72" t="s">
+      <c r="B59" s="68" t="s">
         <v>161</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="73" t="s">
+      <c r="D59" s="69" t="s">
         <v>161</v>
       </c>
       <c r="E59" s="8"/>
-      <c r="F59" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="G59" s="17" t="s">
+      <c r="F59" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="G59" s="58" t="s">
         <v>34</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="24" customHeight="1">
+      <c r="I59" s="58"/>
+    </row>
+    <row r="60" spans="1:10" ht="24" customHeight="1">
       <c r="A60" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B60" s="73" t="s">
+      <c r="B60" s="69" t="s">
         <v>216</v>
       </c>
       <c r="C60" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D60" s="73" t="s">
+      <c r="D60" s="69" t="s">
         <v>225</v>
       </c>
       <c r="E60" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F60" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="G60" s="17" t="s">
+      <c r="F60" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="G60" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="H60" s="17">
+      <c r="H60" s="58">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="24" customHeight="1">
+      <c r="I60" s="58"/>
+    </row>
+    <row r="61" spans="1:10" ht="24" customHeight="1">
       <c r="A61" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B61" s="73" t="s">
+      <c r="B61" s="69" t="s">
         <v>217</v>
       </c>
       <c r="C61" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D61" s="73" t="s">
+      <c r="D61" s="69" t="s">
         <v>226</v>
       </c>
       <c r="E61" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F61" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="G61" s="17" t="s">
+      <c r="F61" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="G61" s="58" t="s">
         <v>35</v>
       </c>
       <c r="H61" s="25">
         <v>480</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="24" customHeight="1">
+      <c r="I61" s="58"/>
+    </row>
+    <row r="62" spans="1:10" ht="24" customHeight="1">
       <c r="A62" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B62" s="73" t="s">
+      <c r="B62" s="69" t="s">
         <v>218</v>
       </c>
       <c r="C62" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D62" s="73" t="s">
+      <c r="D62" s="69" t="s">
         <v>227</v>
       </c>
       <c r="E62" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F62" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="G62" s="17" t="s">
+      <c r="F62" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="G62" s="58" t="s">
         <v>35</v>
       </c>
       <c r="H62" s="25">
         <v>10</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="24" customHeight="1">
+      <c r="I62" s="58"/>
+    </row>
+    <row r="63" spans="1:10" ht="24" customHeight="1">
       <c r="A63" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B63" s="73" t="s">
+      <c r="B63" s="69" t="s">
         <v>219</v>
       </c>
       <c r="C63" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D63" s="73" t="s">
+      <c r="D63" s="69" t="s">
         <v>228</v>
       </c>
       <c r="E63" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="F63" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="G63" s="17" t="s">
+      <c r="F63" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="G63" s="58" t="s">
         <v>35</v>
       </c>
       <c r="H63" s="25">
         <v>340</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="24" customHeight="1">
+      <c r="I63" s="58"/>
+    </row>
+    <row r="64" spans="1:10" ht="24" customHeight="1">
       <c r="A64" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B64" s="73" t="s">
+      <c r="B64" s="69" t="s">
         <v>220</v>
       </c>
       <c r="C64" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D64" s="73" t="s">
+      <c r="D64" s="69" t="s">
         <v>229</v>
       </c>
       <c r="E64" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="F64" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="G64" s="17" t="s">
+      <c r="F64" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="G64" s="58" t="s">
         <v>35</v>
       </c>
       <c r="H64" s="25">
         <v>20</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="24" customHeight="1">
+      <c r="I64" s="58"/>
+    </row>
+    <row r="65" spans="1:10" ht="24" customHeight="1">
       <c r="A65" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B65" s="73" t="s">
+      <c r="B65" s="69" t="s">
         <v>221</v>
       </c>
       <c r="C65" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D65" s="73" t="s">
+      <c r="D65" s="69" t="s">
         <v>230</v>
       </c>
       <c r="E65" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="F65" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="G65" s="17" t="s">
+      <c r="F65" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="G65" s="58" t="s">
         <v>35</v>
       </c>
       <c r="H65" s="25">
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="24" customHeight="1">
+    <row r="66" spans="1:10" ht="24" customHeight="1">
       <c r="A66" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="73" t="s">
+      <c r="B66" s="69" t="s">
         <v>222</v>
       </c>
       <c r="C66" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D66" s="73" t="s">
+      <c r="D66" s="69" t="s">
         <v>231</v>
       </c>
       <c r="E66" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="F66" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="G66" s="17" t="s">
+      <c r="F66" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="G66" s="58" t="s">
         <v>35</v>
       </c>
       <c r="H66" s="25">
@@ -3444,61 +3988,582 @@
         <v>440</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="24" customHeight="1">
+    <row r="67" spans="1:10" ht="24" customHeight="1">
       <c r="A67" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B67" s="72" t="s">
+      <c r="B67" s="68" t="s">
         <v>223</v>
       </c>
       <c r="C67" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D67" s="73" t="s">
+      <c r="D67" s="69" t="s">
         <v>232</v>
       </c>
       <c r="E67" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="F67" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="G67" s="17" t="s">
+      <c r="F67" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="G67" s="58" t="s">
         <v>35</v>
       </c>
       <c r="H67" s="25">
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="24" customHeight="1">
+    <row r="68" spans="1:10" ht="24" customHeight="1">
       <c r="A68" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B68" s="72" t="s">
+      <c r="B68" s="68" t="s">
         <v>224</v>
       </c>
       <c r="C68" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D68" s="73" t="s">
+      <c r="D68" s="69" t="s">
         <v>233</v>
       </c>
       <c r="E68" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="F68" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="G68" s="17" t="s">
+      <c r="F68" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="G68" s="58" t="s">
         <v>35</v>
       </c>
       <c r="H68" s="25">
         <v>363633</v>
       </c>
     </row>
+    <row r="71" spans="1:10" ht="24" customHeight="1">
+      <c r="A71" s="86" t="s">
+        <v>234</v>
+      </c>
+      <c r="B71" s="87"/>
+      <c r="C71" s="87"/>
+      <c r="D71" s="87"/>
+      <c r="E71" s="87"/>
+      <c r="F71" s="87"/>
+      <c r="G71" s="87"/>
+      <c r="H71" s="87"/>
+      <c r="I71" s="87"/>
+      <c r="J71" s="88"/>
+    </row>
+    <row r="72" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A72" s="92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="93" t="s">
+        <v>210</v>
+      </c>
+      <c r="C72" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="93" t="s">
+        <v>209</v>
+      </c>
+      <c r="E72" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="F72" s="93" t="s">
+        <v>213</v>
+      </c>
+      <c r="G72" s="93" t="s">
+        <v>7</v>
+      </c>
+      <c r="H72" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="I72" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J72" s="94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A73" s="76" t="s">
+        <v>235</v>
+      </c>
+      <c r="B73" s="95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C73" s="76" t="s">
+        <v>237</v>
+      </c>
+      <c r="D73" s="75" t="s">
+        <v>236</v>
+      </c>
+      <c r="E73" s="77" t="s">
+        <v>238</v>
+      </c>
+      <c r="F73" s="96" t="s">
+        <v>211</v>
+      </c>
+      <c r="G73" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="H73" s="94" t="s">
+        <v>239</v>
+      </c>
+      <c r="I73" s="78" t="s">
+        <v>240</v>
+      </c>
+      <c r="J73" s="94"/>
+    </row>
+    <row r="74" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A74" s="76" t="s">
+        <v>241</v>
+      </c>
+      <c r="B74" s="95" t="s">
+        <v>242</v>
+      </c>
+      <c r="C74" s="76" t="s">
+        <v>243</v>
+      </c>
+      <c r="D74" s="75" t="s">
+        <v>244</v>
+      </c>
+      <c r="E74" s="77" t="s">
+        <v>238</v>
+      </c>
+      <c r="F74" s="96" t="s">
+        <v>211</v>
+      </c>
+      <c r="G74" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="H74" s="94" t="s">
+        <v>245</v>
+      </c>
+      <c r="I74" s="79" t="s">
+        <v>246</v>
+      </c>
+      <c r="J74" s="94"/>
+    </row>
+    <row r="75" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A75" s="76" t="s">
+        <v>247</v>
+      </c>
+      <c r="B75" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="C75" s="76" t="s">
+        <v>249</v>
+      </c>
+      <c r="D75" s="75" t="s">
+        <v>248</v>
+      </c>
+      <c r="E75" s="77" t="s">
+        <v>238</v>
+      </c>
+      <c r="F75" s="96" t="s">
+        <v>211</v>
+      </c>
+      <c r="G75" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H75" s="94">
+        <v>93</v>
+      </c>
+      <c r="I75" s="93"/>
+      <c r="J75" s="94"/>
+    </row>
+    <row r="76" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A76" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="B76" s="95" t="s">
+        <v>252</v>
+      </c>
+      <c r="C76" s="76" t="s">
+        <v>253</v>
+      </c>
+      <c r="D76" s="75" t="s">
+        <v>252</v>
+      </c>
+      <c r="E76" s="77" t="s">
+        <v>238</v>
+      </c>
+      <c r="F76" s="96" t="s">
+        <v>211</v>
+      </c>
+      <c r="G76" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="H76" s="94" t="s">
+        <v>254</v>
+      </c>
+      <c r="I76" s="80" t="s">
+        <v>255</v>
+      </c>
+      <c r="J76" s="94"/>
+    </row>
+    <row r="77" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A77" s="76" t="s">
+        <v>256</v>
+      </c>
+      <c r="B77" s="95" t="s">
+        <v>257</v>
+      </c>
+      <c r="C77" s="76" t="s">
+        <v>258</v>
+      </c>
+      <c r="D77" s="75" t="s">
+        <v>259</v>
+      </c>
+      <c r="E77" s="81" t="s">
+        <v>260</v>
+      </c>
+      <c r="F77" s="96" t="s">
+        <v>211</v>
+      </c>
+      <c r="G77" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H77" s="61" t="s">
+        <v>261</v>
+      </c>
+      <c r="I77" s="82"/>
+      <c r="J77" s="82"/>
+    </row>
+    <row r="78" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A78" s="76" t="s">
+        <v>262</v>
+      </c>
+      <c r="B78" s="61" t="s">
+        <v>263</v>
+      </c>
+      <c r="C78" s="76" t="s">
+        <v>264</v>
+      </c>
+      <c r="D78" s="75" t="s">
+        <v>265</v>
+      </c>
+      <c r="E78" s="81" t="s">
+        <v>260</v>
+      </c>
+      <c r="F78" s="96" t="s">
+        <v>211</v>
+      </c>
+      <c r="G78" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H78" s="61" t="s">
+        <v>266</v>
+      </c>
+      <c r="I78" s="82"/>
+      <c r="J78" s="82"/>
+    </row>
+    <row r="79" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A79" s="76" t="s">
+        <v>267</v>
+      </c>
+      <c r="B79" s="61" t="s">
+        <v>268</v>
+      </c>
+      <c r="C79" s="76" t="s">
+        <v>269</v>
+      </c>
+      <c r="D79" s="75" t="s">
+        <v>270</v>
+      </c>
+      <c r="E79" s="81" t="s">
+        <v>260</v>
+      </c>
+      <c r="F79" s="96" t="s">
+        <v>211</v>
+      </c>
+      <c r="G79" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H79" s="61" t="s">
+        <v>271</v>
+      </c>
+      <c r="I79" s="82"/>
+      <c r="J79" s="82"/>
+    </row>
+    <row r="80" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A80" s="76" t="s">
+        <v>272</v>
+      </c>
+      <c r="B80" s="95" t="s">
+        <v>273</v>
+      </c>
+      <c r="C80" s="76" t="s">
+        <v>274</v>
+      </c>
+      <c r="D80" s="75" t="s">
+        <v>275</v>
+      </c>
+      <c r="E80" s="83" t="s">
+        <v>276</v>
+      </c>
+      <c r="F80" s="96" t="s">
+        <v>211</v>
+      </c>
+      <c r="G80" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H80" s="61" t="s">
+        <v>277</v>
+      </c>
+      <c r="I80" s="82"/>
+      <c r="J80" s="82"/>
+    </row>
+    <row r="81" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A81" s="76" t="s">
+        <v>278</v>
+      </c>
+      <c r="B81" s="95" t="s">
+        <v>279</v>
+      </c>
+      <c r="C81" s="76" t="s">
+        <v>280</v>
+      </c>
+      <c r="D81" s="75" t="s">
+        <v>281</v>
+      </c>
+      <c r="E81" s="83" t="s">
+        <v>276</v>
+      </c>
+      <c r="F81" s="96" t="s">
+        <v>211</v>
+      </c>
+      <c r="G81" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H81" s="61" t="s">
+        <v>282</v>
+      </c>
+      <c r="I81" s="82"/>
+      <c r="J81" s="82"/>
+    </row>
+    <row r="82" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A82" s="76" t="s">
+        <v>283</v>
+      </c>
+      <c r="B82" s="95" t="s">
+        <v>284</v>
+      </c>
+      <c r="C82" s="76" t="s">
+        <v>285</v>
+      </c>
+      <c r="D82" s="75" t="s">
+        <v>286</v>
+      </c>
+      <c r="E82" s="83" t="s">
+        <v>276</v>
+      </c>
+      <c r="F82" s="96" t="s">
+        <v>211</v>
+      </c>
+      <c r="G82" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H82" s="61" t="s">
+        <v>287</v>
+      </c>
+      <c r="I82" s="82"/>
+      <c r="J82" s="82"/>
+    </row>
+    <row r="83" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A83" s="76" t="s">
+        <v>288</v>
+      </c>
+      <c r="B83" s="95" t="s">
+        <v>289</v>
+      </c>
+      <c r="C83" s="76" t="s">
+        <v>290</v>
+      </c>
+      <c r="D83" s="75" t="s">
+        <v>291</v>
+      </c>
+      <c r="E83" s="84" t="s">
+        <v>292</v>
+      </c>
+      <c r="F83" s="96" t="s">
+        <v>212</v>
+      </c>
+      <c r="G83" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H83" s="61" t="s">
+        <v>293</v>
+      </c>
+      <c r="I83" s="82"/>
+      <c r="J83" s="82"/>
+    </row>
+    <row r="84" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A84" s="76" t="s">
+        <v>294</v>
+      </c>
+      <c r="B84" s="95" t="s">
+        <v>295</v>
+      </c>
+      <c r="C84" s="76" t="s">
+        <v>296</v>
+      </c>
+      <c r="D84" s="75" t="s">
+        <v>297</v>
+      </c>
+      <c r="E84" s="84" t="s">
+        <v>292</v>
+      </c>
+      <c r="F84" s="96" t="s">
+        <v>212</v>
+      </c>
+      <c r="G84" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H84" s="61" t="s">
+        <v>266</v>
+      </c>
+      <c r="I84" s="82"/>
+      <c r="J84" s="82"/>
+    </row>
+    <row r="85" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A85" s="76" t="s">
+        <v>298</v>
+      </c>
+      <c r="B85" s="95" t="s">
+        <v>299</v>
+      </c>
+      <c r="C85" s="76" t="s">
+        <v>300</v>
+      </c>
+      <c r="D85" s="75" t="s">
+        <v>301</v>
+      </c>
+      <c r="E85" s="84" t="s">
+        <v>292</v>
+      </c>
+      <c r="F85" s="96" t="s">
+        <v>212</v>
+      </c>
+      <c r="G85" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H85" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="I85" s="82"/>
+      <c r="J85" s="82"/>
+    </row>
+    <row r="86" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A86" s="76" t="s">
+        <v>303</v>
+      </c>
+      <c r="B86" s="95" t="s">
+        <v>304</v>
+      </c>
+      <c r="C86" s="76" t="s">
+        <v>305</v>
+      </c>
+      <c r="D86" s="75" t="s">
+        <v>306</v>
+      </c>
+      <c r="E86" s="85" t="s">
+        <v>307</v>
+      </c>
+      <c r="F86" s="96" t="s">
+        <v>212</v>
+      </c>
+      <c r="G86" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H86" s="61"/>
+      <c r="I86" s="82"/>
+      <c r="J86" s="82"/>
+    </row>
+    <row r="87" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A87" s="76" t="s">
+        <v>308</v>
+      </c>
+      <c r="B87" s="95" t="s">
+        <v>309</v>
+      </c>
+      <c r="C87" s="76" t="s">
+        <v>310</v>
+      </c>
+      <c r="D87" s="75" t="s">
+        <v>311</v>
+      </c>
+      <c r="E87" s="85" t="s">
+        <v>307</v>
+      </c>
+      <c r="F87" s="96" t="s">
+        <v>212</v>
+      </c>
+      <c r="G87" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H87" s="61"/>
+      <c r="I87" s="82"/>
+      <c r="J87" s="82"/>
+    </row>
+    <row r="88" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A88" s="76" t="s">
+        <v>312</v>
+      </c>
+      <c r="B88" s="95" t="s">
+        <v>313</v>
+      </c>
+      <c r="C88" s="76" t="s">
+        <v>314</v>
+      </c>
+      <c r="D88" s="75" t="s">
+        <v>315</v>
+      </c>
+      <c r="E88" s="85" t="s">
+        <v>307</v>
+      </c>
+      <c r="F88" s="96" t="s">
+        <v>212</v>
+      </c>
+      <c r="G88" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H88" s="61"/>
+      <c r="I88" s="61"/>
+      <c r="J88" s="61"/>
+    </row>
+    <row r="89" spans="1:10" s="56" customFormat="1" ht="24" customHeight="1">
+      <c r="A89" s="76" t="s">
+        <v>316</v>
+      </c>
+      <c r="B89" s="95" t="s">
+        <v>317</v>
+      </c>
+      <c r="C89" s="76" t="s">
+        <v>318</v>
+      </c>
+      <c r="D89" s="75" t="s">
+        <v>319</v>
+      </c>
+      <c r="E89" s="85" t="s">
+        <v>307</v>
+      </c>
+      <c r="F89" s="96" t="s">
+        <v>212</v>
+      </c>
+      <c r="G89" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="H89" s="61"/>
+      <c r="I89" s="61"/>
+      <c r="J89" s="61"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Bg06WcxL6wAS7CfgpDtN4Pd79Zxp8TvVJSgDxYzQJWD5S7wkJm630nwFwOgtBrz6nTcqHcI1051klNT/wq/pKA==" saltValue="GGPcfXjmITwzml+HR+9WeA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="5">
+  <sheetProtection algorithmName="SHA-512" hashValue="eeWmjXtWJZWQajfRgsOr0h9P6Ck/Z0FibqixFdesXFkp0fdeFBMX/toa1VIBf5GD0RT8ZhsiHVyl8vusMg8NwA==" saltValue="kLB8iwQmEgjmKU2tJL6jpQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="6">
+    <mergeCell ref="A71:J71"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
@@ -3511,6 +4576,176 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10094029-CEF1-8F4A-9457-0DA836CB96AD}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="35.6640625" defaultRowHeight="31" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" style="100"/>
+    <col min="2" max="2" width="121.5" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="35.6640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="31" customHeight="1">
+      <c r="A1" s="97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="99" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="31" customHeight="1">
+      <c r="A2" s="98" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" s="101"/>
+    </row>
+    <row r="3" spans="1:2" ht="31" customHeight="1">
+      <c r="A3" s="98" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" s="101"/>
+    </row>
+    <row r="4" spans="1:2" ht="31" customHeight="1">
+      <c r="A4" s="98" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="101"/>
+    </row>
+    <row r="5" spans="1:2" ht="31" customHeight="1">
+      <c r="A5" s="98" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5" s="101"/>
+    </row>
+    <row r="6" spans="1:2" ht="31" customHeight="1">
+      <c r="A6" s="98" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" s="102"/>
+    </row>
+    <row r="7" spans="1:2" ht="31" customHeight="1">
+      <c r="A7" s="98" t="s">
+        <v>262</v>
+      </c>
+      <c r="B7" s="103"/>
+    </row>
+    <row r="8" spans="1:2" ht="31" customHeight="1">
+      <c r="A8" s="98" t="s">
+        <v>267</v>
+      </c>
+      <c r="B8" s="103"/>
+    </row>
+    <row r="9" spans="1:2" ht="31" customHeight="1">
+      <c r="A9" s="98" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="102"/>
+    </row>
+    <row r="10" spans="1:2" ht="31" customHeight="1">
+      <c r="A10" s="98" t="s">
+        <v>278</v>
+      </c>
+      <c r="B10" s="102"/>
+    </row>
+    <row r="11" spans="1:2" ht="31" customHeight="1">
+      <c r="A11" s="98" t="s">
+        <v>283</v>
+      </c>
+      <c r="B11" s="102"/>
+    </row>
+    <row r="12" spans="1:2" ht="31" customHeight="1">
+      <c r="A12" s="98" t="s">
+        <v>288</v>
+      </c>
+      <c r="B12" s="102"/>
+    </row>
+    <row r="13" spans="1:2" ht="31" customHeight="1">
+      <c r="A13" s="98" t="s">
+        <v>294</v>
+      </c>
+      <c r="B13" s="102"/>
+    </row>
+    <row r="14" spans="1:2" ht="31" customHeight="1">
+      <c r="A14" s="98" t="s">
+        <v>298</v>
+      </c>
+      <c r="B14" s="102"/>
+    </row>
+    <row r="15" spans="1:2" ht="31" customHeight="1">
+      <c r="A15" s="98" t="s">
+        <v>303</v>
+      </c>
+      <c r="B15" s="102"/>
+    </row>
+    <row r="16" spans="1:2" ht="31" customHeight="1">
+      <c r="A16" s="98" t="s">
+        <v>308</v>
+      </c>
+      <c r="B16" s="102"/>
+    </row>
+    <row r="17" spans="1:2" ht="31" customHeight="1">
+      <c r="A17" s="98" t="s">
+        <v>312</v>
+      </c>
+      <c r="B17" s="102"/>
+    </row>
+    <row r="18" spans="1:2" ht="31" customHeight="1">
+      <c r="A18" s="98" t="s">
+        <v>316</v>
+      </c>
+      <c r="B18" s="102"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="HuQ4UPofJyEVo1SSitMiy9ccUV6amLxZUbxGHfvXb1Kv+3F9PBgVhSduAWr/p7i4sShsw9s5GPvxdwP7PvBEdQ==" saltValue="hH/VhhveBHOo4x/vJrG0lg==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <dataValidations count="30">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="参考基因组" prompt="GRCh38 (hg38)" sqref="A2" xr:uid="{116B740B-4A22-B14D-AD48-FB5E06915D18}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="参考基因组" sqref="B2" xr:uid="{C0605E7B-14B8-754B-98A6-E7BCC45DA800}">
+      <formula1>"GRCh38 (hg38)"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="基因模型来源" prompt="例如：Ensembl, UCSC, RefSeq等，基因模型文件通常是gtf/gff格式" sqref="A3" xr:uid="{ED01F829-7C94-9C42-9EF6-134B09C77B26}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="基因模型来源" sqref="B3" xr:uid="{F9E29E47-CEB0-5944-BD9E-A7C4D1756617}">
+      <formula1>"Ensembl,UCSC,RefSeq,GENCODE,Other"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="基因注释版本" sqref="A4" xr:uid="{3F44071C-0AB2-1949-AE28-9A96A3FD7DAE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="基因注释版本" prompt="例如：93" sqref="B4" xr:uid="{563F918F-E71C-6941-89B0-C47F9C88725E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="基因名种类" prompt="例如：Ensembl ID, HGNC symbol, Entrez ID, other" sqref="A5" xr:uid="{1C718A79-B817-F44B-8105-9507EAF44503}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{54647A50-122D-F742-9DCC-CE513CE87ADE}">
+      <formula1>"Ensembl ID, HGNC symbol, Entrez ID, other"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="比对软件" prompt="用于将序列比对至参考基因组软件，如果使用多个比对软件，则用分号分隔 (;)" sqref="A6" xr:uid="{38ED9164-C02F-6C44-BFDD-85BDB9D732E9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="例如：HISAT2" sqref="B6" xr:uid="{76A05FB0-EDFC-FB4B-8A6D-A14D9D9FDB39}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="比对软件版本号" prompt="如果使用多个比对软件，则用分号分隔 (;)" sqref="A7" xr:uid="{AE367543-859F-CE4F-A5E8-B0F2EEB388DA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="比对软件版本号" prompt="例如：v0.11.5" sqref="B7" xr:uid="{C12430CF-152B-2A44-8FAE-3633E77E83C9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="比对运行命令行" prompt="如果使用多行命令，则用分号分隔 (;)" sqref="A8" xr:uid="{44D36704-B84D-2748-AFA7-6802F8BE149C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="hisat2 -p 8 -x reference/References_GRCh38/GRCh38/ -1 sample_R1.fastq.gz -2 sample_R2.fastq.gz -S sample.sam " sqref="B8" xr:uid="{8BB0F008-06F2-A743-9C3D-670C8A37DBAC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="定量软件" prompt="如果使用多个软件，则用分号分隔 (;)" sqref="A9" xr:uid="{50C64189-1262-2C47-865C-98141A9D8C9B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="例如：StringTie" sqref="B9" xr:uid="{3592F2EA-6105-9F4E-9E7D-867615D24B02}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="定量软件版本号，如果使用多个软件，则用分号分隔 (;)" sqref="A10" xr:uid="{FF86F5DF-5B1A-A541-8406-D9CAF1AF01BD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="例如：v1.3.4" sqref="B10" xr:uid="{A1236B87-9475-A94C-AE2D-AF5A2EB28C38}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="定量软件命令行，如果使用多个软件，则用分号分隔 (;)" sqref="A11" xr:uid="{0C413F54-23AE-C447-BDEF-16C1BF95CBB2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="stringtie -e -B -p 8 -G Homo_sapiens.GRCh38.93.gtf  -g sample_genecount.csv -o sample.gtf -C sample.cov.ref.gtf -A sample.gene.abundance.txt sample.sorted.bam" sqref="B11" xr:uid="{7BAC2291-E570-CA4D-86BB-326C643AD30E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="质控软件，如果使用多个软件，则用分号分隔 (;)" sqref="A12" xr:uid="{364377AA-749E-7943-AA6D-E5D32E07BB8A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="例如：FastQC" sqref="B12" xr:uid="{C910C86D-5984-3D4F-8AA7-2F0D26129638}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="质控软件版本号，如果使用多个软件，则用分号分隔 (;)" sqref="A13" xr:uid="{1FBBDEB3-18B6-594D-9CA7-8859E2D4D9ED}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="例如：v0.11.5" sqref="B13" xr:uid="{BE9FD74A-7CD2-BD40-96FB-A0DCB1CBC8A4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="质控软件命令行，如果使用多个软件，则用分号分隔 (;)" sqref="A14" xr:uid="{2D93B087-BCC4-D04A-97BC-9BBB8303D566}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="例如：fastqc –o outdir sample.fastq.gz" sqref="B14" xr:uid="{08CCDF34-2320-304C-A184-02B0FD15CEE1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="其它软件，如果使用多个软件，则用分号分隔 (;)" sqref="A15" xr:uid="{B47088CC-249F-D14A-B23E-596CD223E98A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="其它软件用途，如果使用多个软件，则用分号分隔 (;)" sqref="A16" xr:uid="{99210146-480A-AB4A-9D8C-81DA6E820E27}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="其它软件版本号，如果使用多个软件，则用分号分隔 (;)" sqref="A17" xr:uid="{8DDD5C72-A367-F446-9C7B-7BFE0584646C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="其它软件命令行，如果使用多个软件，则用分号分隔 (;)" sqref="A18" xr:uid="{3B3BC51A-06A3-B047-82EE-5FE01BCB2955}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECE994F-BB82-2E4E-84AB-792F6F7C8F43}">
   <dimension ref="A1:AW1"/>
   <sheetViews>
@@ -3685,7 +4920,7 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="4LfHwKMQ2qyoY+hz+Xhfs2yd4xpmEFyzEpNaO0oBp+/coBGUb5M+PGe97dZcW43IiuG/5r1IzQTwrHR2SEJQlg==" saltValue="35X+smEeBsDqerS5gAh6jw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <dataValidations count="94">
+  <dataValidations count="93">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="&lt;lab-name&gt;_Illumina_D5_&lt;sequencing-date&gt;_&lt;no.&gt;_R1/R2.fastq.gz_x000d__x000a__x000d__x000a_e.g FDU_Illumina_D5_20200808_001_R1.fastq.gz" sqref="B2:B1048576" xr:uid="{EE4EBFB8-3AF4-9545-A3BA-CB54EA5CFE04}"/>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="File Size (Bytes)" prompt="e.g. 10000000" sqref="C2:C1048576" xr:uid="{8A72CF26-BFC1-FE48-803A-C8B88DD253C8}">
       <formula1>0</formula1>
@@ -3803,7 +5038,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="RNA打断温度（℃）" prompt="例如：85" sqref="O1" xr:uid="{3844C213-F51A-0841-B1B3-46DF314EC4F2}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="RNA打断时间（分钟）" prompt="例如：5" sqref="P1" xr:uid="{56E5ED8B-7FED-6449-B7CD-472E9E96901F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="RNA富集操作日期" prompt="例如：20200808" sqref="Q1" xr:uid="{AFB57773-8450-0549-B784-FF926DC9E982}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="自动化或手动操作" prompt="例如：Manual或Automated" sqref="R1" xr:uid="{1B5C5999-BBA8-E242-B24C-56ECFB499633}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="自动化或手动操作" prompt="例如：Manual或Automated" sqref="R1 AL1" xr:uid="{1B5C5999-BBA8-E242-B24C-56ECFB499633}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="是否为链特异性文库" prompt="例如：TRUE或FALSE" sqref="S1" xr:uid="{E360AFD5-F14D-9146-83C3-DD6D3E05BF1D}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="建库试剂盒品牌" prompt="例如：Vazyme" sqref="T1" xr:uid="{696FC65F-FC91-9A4F-9A38-CCC304B31837}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="建库试剂盒名称" prompt="例如：VAHTS Universal V8 RNA-seq Library Prep Kit for Illumina" sqref="U1" xr:uid="{39360DE6-42FF-4743-88A3-EBB1B47A87BD}"/>
@@ -3823,7 +5058,6 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="片段筛选第二轮磁珠用量（uL）" prompt="例如：7.5" sqref="AI1" xr:uid="{4F08F823-B1AF-8940-B8F3-71780D60061D}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="PCR循环数" prompt="例如：15" sqref="AJ1" xr:uid="{07379FF3-00CD-4947-B953-6AE287916738}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="文库制备操作日期" prompt="例如：20200808" sqref="AK1" xr:uid="{7709B4E5-B7B7-3248-AF0F-D99AC02E1F2D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="自动化或手动操作" prompt="例如：Manual或Automated" sqref="AL1" xr:uid="{A7F43F4A-608F-CA47-997E-1B4748183542}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="测序平台" prompt="例如：Illumina或MGI" sqref="AM1" xr:uid="{CAEA06BE-C09A-1C49-87ED-67FBB8D39517}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="测序仪器" prompt="例如：NovaSeq 6000" sqref="AN1" xr:uid="{A44D2127-F2D8-E44B-B097-A4EA134D0178}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="测序模式" prompt="例如：PE150" sqref="AO1" xr:uid="{BF57752D-CA44-A744-AFD3-A0486899AA57}"/>
@@ -3841,11 +5075,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EA9666-A0F9-934D-B4B5-980441048860}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>

</xml_diff>